<commit_message>
RLWS 1.3; cables for 24V
</commit_message>
<xml_diff>
--- a/Docs/AT-ETX-2i10G.CBL11.xlsx
+++ b/Docs/AT-ETX-2i10G.CBL11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2i-10G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6DD57D-0E29-45AE-8BEE-C986723979F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AFD902-29AC-48C2-9D60-62B1CE8816F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="1455" windowWidth="20895" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2325" yWindow="1320" windowWidth="21600" windowHeight="13845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,11 +163,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,10 +521,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -653,7 +653,7 @@
       <c r="D21" s="4"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>